<commit_message>
time stamp before cleanup
</commit_message>
<xml_diff>
--- a/notebooks/reflection_messages/table_3.xlsx
+++ b/notebooks/reflection_messages/table_3.xlsx
@@ -457,170 +457,170 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>66.87830687830687</v>
+        <v>89.68085106382979</v>
       </c>
       <c r="B2" t="n">
-        <v>59.64630225080386</v>
+        <v>87.36196319018404</v>
       </c>
       <c r="C2" t="n">
-        <v>7.232004627503017</v>
+        <v>2.31888787364575</v>
       </c>
       <c r="D2" t="n">
-        <v>0.015</v>
+        <v>0.022</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>65.37037037037037</v>
+        <v>95.80851063829788</v>
       </c>
       <c r="B3" t="n">
-        <v>60.77170418006431</v>
+        <v>94.66257668711657</v>
       </c>
       <c r="C3" t="n">
-        <v>4.598666190306055</v>
+        <v>1.145933951181306</v>
       </c>
       <c r="D3" t="n">
-        <v>0.073</v>
+        <v>0.044</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>45.76719576719577</v>
+        <v>91.02127659574468</v>
       </c>
       <c r="B4" t="n">
-        <v>32.90996784565916</v>
+        <v>88.83435582822086</v>
       </c>
       <c r="C4" t="n">
-        <v>12.85722792153661</v>
+        <v>2.186920767523816</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>0.019</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>46.95767195767196</v>
+        <v>89.02127659574468</v>
       </c>
       <c r="B5" t="n">
-        <v>36.52733118971061</v>
+        <v>85.42944785276073</v>
       </c>
       <c r="C5" t="n">
-        <v>10.43034076796135</v>
+        <v>3.591828742983949</v>
       </c>
       <c r="D5" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>48.80952380952381</v>
+        <v>83.1063829787234</v>
       </c>
       <c r="B6" t="n">
-        <v>41.27009646302251</v>
+        <v>80.30674846625767</v>
       </c>
       <c r="C6" t="n">
-        <v>7.539427346501299</v>
+        <v>2.79963451246573</v>
       </c>
       <c r="D6" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.025</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>46.24338624338624</v>
+        <v>86.06382978723404</v>
       </c>
       <c r="B7" t="n">
-        <v>35.20900321543408</v>
+        <v>83.61963190184049</v>
       </c>
       <c r="C7" t="n">
-        <v>11.03438302795216</v>
+        <v>2.44419788539355</v>
       </c>
       <c r="D7" t="n">
-        <v>0.001</v>
+        <v>0.017</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>44.41798941798942</v>
+        <v>85.04255319148936</v>
       </c>
       <c r="B8" t="n">
-        <v>34.08360128617363</v>
+        <v>82.20858895705521</v>
       </c>
       <c r="C8" t="n">
-        <v>10.33438813181579</v>
+        <v>2.833964234434148</v>
       </c>
       <c r="D8" t="n">
-        <v>0.002</v>
+        <v>0.019</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>51.37566137566137</v>
+        <v>92.42553191489361</v>
       </c>
       <c r="B9" t="n">
-        <v>37.491961414791</v>
+        <v>90.06134969325153</v>
       </c>
       <c r="C9" t="n">
-        <v>13.88369996087037</v>
+        <v>2.364182221642082</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>0.004</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>37.53968253968254</v>
+        <v>77.93617021276596</v>
       </c>
       <c r="B10" t="n">
-        <v>25.4983922829582</v>
+        <v>75.30674846625767</v>
       </c>
       <c r="C10" t="n">
-        <v>12.04129025672434</v>
+        <v>2.629421746508285</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>48.22751322751323</v>
+        <v>87.82978723404256</v>
       </c>
       <c r="B11" t="n">
-        <v>35.32154340836013</v>
+        <v>85.2760736196319</v>
       </c>
       <c r="C11" t="n">
-        <v>12.9059698191531</v>
+        <v>2.553713614410654</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>50.31746031746032</v>
+        <v>96.17021276595744</v>
       </c>
       <c r="B12" t="n">
-        <v>36.20578778135048</v>
+        <v>93.12883435582822</v>
       </c>
       <c r="C12" t="n">
-        <v>14.11167253610984</v>
+        <v>3.041378410129226</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>50.17316017316016</v>
+        <v>88.55512572533848</v>
       </c>
       <c r="B13" t="n">
-        <v>39.53960830166618</v>
+        <v>86.01784718349136</v>
       </c>
       <c r="C13" t="n">
-        <v>10.63355187149398</v>
+        <v>2.53727854184713</v>
       </c>
       <c r="D13" t="n">
-        <v>0.002</v>
+        <v>0.003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>